<commit_message>
updates to code prototype
</commit_message>
<xml_diff>
--- a/qual/data/AFG_asylum-decisions_TEST.xlsx
+++ b/qual/data/AFG_asylum-decisions_TEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tatianakalainoff/Documents/GitHub/major-studio/qual/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FBF561-BEEE-C445-BB06-933B8C106460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07763C65-FC8C-F94C-A6FC-4059004DA740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="asylum-decisions" sheetId="1" r:id="rId1"/>
@@ -1511,16 +1511,16 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q616"/>
   <sheetViews>
-    <sheetView zoomScale="59" workbookViewId="0">
-      <selection activeCell="D614" sqref="D614"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T533" sqref="T533"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="9.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="4.33203125" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="6.1640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="4.5" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="12" width="11.33203125" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
     <col min="14" max="14" width="13.1640625" customWidth="1"/>
@@ -23165,7 +23165,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="516" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A516">
         <v>2021</v>
       </c>
@@ -23182,7 +23182,7 @@
         <v>27</v>
       </c>
       <c r="F516" s="3">
-        <f>SUM(Q516/129293)</f>
+        <f t="shared" ref="F516:F547" si="0">SUM(Q516/129293)</f>
         <v>7.165121081574409E-2</v>
       </c>
       <c r="G516" t="s">
@@ -23221,7 +23221,7 @@
         <v>9264</v>
       </c>
     </row>
-    <row r="517" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="517" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A517">
         <v>2021</v>
       </c>
@@ -23238,7 +23238,7 @@
         <v>32</v>
       </c>
       <c r="F517" s="3">
-        <f>SUM(Q517/129293)</f>
+        <f t="shared" si="0"/>
         <v>1.8253115017827726E-2</v>
       </c>
       <c r="G517" t="s">
@@ -23254,7 +23254,7 @@
         <v>815</v>
       </c>
       <c r="K517" s="3">
-        <f t="shared" ref="K517:K538" si="0">SUM(J517/$J$615)</f>
+        <f t="shared" ref="K517:K538" si="1">SUM(J517/$J$615)</f>
         <v>2.2448698526373777E-2</v>
       </c>
       <c r="L517" s="4">
@@ -23264,7 +23264,7 @@
         <v>355</v>
       </c>
       <c r="N517" s="3">
-        <f t="shared" ref="N517:N538" si="1">SUM(M517/$M$615)</f>
+        <f t="shared" ref="N517:N538" si="2">SUM(M517/$M$615)</f>
         <v>1.2017603249830738E-2</v>
       </c>
       <c r="O517">
@@ -23277,7 +23277,7 @@
         <v>2360</v>
       </c>
     </row>
-    <row r="518" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="518" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A518">
         <v>2021</v>
       </c>
@@ -23294,7 +23294,7 @@
         <v>41</v>
       </c>
       <c r="F518" s="3">
-        <f>SUM(Q518/129293)</f>
+        <f t="shared" si="0"/>
         <v>2.2940143704608913E-2</v>
       </c>
       <c r="G518" t="s">
@@ -23320,7 +23320,7 @@
         <v>33</v>
       </c>
       <c r="N518" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.117129316181449E-3</v>
       </c>
       <c r="O518">
@@ -23333,7 +23333,7 @@
         <v>2966</v>
       </c>
     </row>
-    <row r="519" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="519" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A519">
         <v>2021</v>
       </c>
@@ -23350,7 +23350,7 @@
         <v>70</v>
       </c>
       <c r="F519" s="3">
-        <f>SUM(Q519/129293)</f>
+        <f t="shared" si="0"/>
         <v>1.2189368333939193E-2</v>
       </c>
       <c r="G519" t="s">
@@ -23366,7 +23366,7 @@
         <v>40</v>
       </c>
       <c r="K519" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1017766147913511E-3</v>
       </c>
       <c r="L519" s="4">
@@ -23376,7 +23376,7 @@
         <v>0</v>
       </c>
       <c r="N519" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O519">
@@ -23389,7 +23389,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="520" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="520" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A520">
         <v>2021</v>
       </c>
@@ -23406,7 +23406,7 @@
         <v>59</v>
       </c>
       <c r="F520" s="3">
-        <f>SUM(Q520/129293)</f>
+        <f t="shared" si="0"/>
         <v>0.12697516493545669</v>
       </c>
       <c r="G520" t="s">
@@ -23422,18 +23422,18 @@
         <v>4611</v>
       </c>
       <c r="K520" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.12700729927007298</v>
       </c>
       <c r="L520" s="4">
-        <f t="shared" ref="L517:L538" si="2">SUM(280*K520)</f>
+        <f t="shared" ref="L520:L537" si="3">SUM(280*K520)</f>
         <v>35.562043795620433</v>
       </c>
       <c r="M520">
         <v>7625</v>
       </c>
       <c r="N520" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25812457684495599</v>
       </c>
       <c r="O520">
@@ -23446,7 +23446,7 @@
         <v>16417</v>
       </c>
     </row>
-    <row r="521" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A521">
         <v>2021</v>
       </c>
@@ -23463,7 +23463,7 @@
         <v>59</v>
       </c>
       <c r="F521" s="3">
-        <f>SUM(Q521/129293)</f>
+        <f t="shared" si="0"/>
         <v>3.4619043567710547E-2</v>
       </c>
       <c r="G521" t="s">
@@ -23479,7 +23479,7 @@
         <v>958</v>
       </c>
       <c r="K521" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.6387549924252858E-2</v>
       </c>
       <c r="L521" s="4">
@@ -23489,7 +23489,7 @@
         <v>2037</v>
       </c>
       <c r="N521" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.8957345971563985E-2</v>
       </c>
       <c r="O521">
@@ -23502,7 +23502,7 @@
         <v>4476</v>
       </c>
     </row>
-    <row r="522" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="522" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A522">
         <v>2021</v>
       </c>
@@ -23519,7 +23519,7 @@
         <v>65</v>
       </c>
       <c r="F522" s="3">
-        <f>SUM(Q522/129293)</f>
+        <f t="shared" si="0"/>
         <v>0.12586914991530865</v>
       </c>
       <c r="G522" t="s">
@@ -23535,7 +23535,7 @@
         <v>979</v>
       </c>
       <c r="K522" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.6965982647018317E-2</v>
       </c>
       <c r="L522" s="4">
@@ -23545,7 +23545,7 @@
         <v>6870</v>
       </c>
       <c r="N522" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.23256601218686526</v>
       </c>
       <c r="O522">
@@ -23558,7 +23558,7 @@
         <v>16274</v>
       </c>
     </row>
-    <row r="523" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="523" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A523">
         <v>2021</v>
       </c>
@@ -23575,7 +23575,7 @@
         <v>65</v>
       </c>
       <c r="F523" s="3">
-        <f>SUM(Q523/129293)</f>
+        <f t="shared" si="0"/>
         <v>6.2694809463776077E-2</v>
       </c>
       <c r="G523" t="s">
@@ -23591,7 +23591,7 @@
         <v>1409</v>
       </c>
       <c r="K523" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8810081256025343E-2</v>
       </c>
       <c r="L523" s="4">
@@ -23601,7 +23601,7 @@
         <v>2233</v>
       </c>
       <c r="N523" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.5592417061611378E-2</v>
       </c>
       <c r="O523">
@@ -23614,7 +23614,7 @@
         <v>8106</v>
       </c>
     </row>
-    <row r="524" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="524" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A524">
         <v>2021</v>
       </c>
@@ -23631,7 +23631,7 @@
         <v>65</v>
       </c>
       <c r="F524" s="3">
-        <f>SUM(Q524/129293)</f>
+        <f t="shared" si="0"/>
         <v>1.4996944923545745E-2</v>
       </c>
       <c r="G524" t="s">
@@ -23647,7 +23647,7 @@
         <v>166</v>
       </c>
       <c r="K524" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.5723729513841068E-3</v>
       </c>
       <c r="L524" s="4">
@@ -23657,7 +23657,7 @@
         <v>500</v>
       </c>
       <c r="N524" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6926201760324982E-2</v>
       </c>
       <c r="O524">
@@ -23670,7 +23670,7 @@
         <v>1939</v>
       </c>
     </row>
-    <row r="525" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="525" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A525">
         <v>2021</v>
       </c>
@@ -23687,7 +23687,7 @@
         <v>68</v>
       </c>
       <c r="F525" s="3">
-        <f>SUM(Q525/129293)</f>
+        <f t="shared" si="0"/>
         <v>0.12364165113347203</v>
       </c>
       <c r="G525" t="s">
@@ -23703,18 +23703,18 @@
         <v>4235</v>
       </c>
       <c r="K525" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1166505990910343</v>
       </c>
       <c r="L525" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32.662167745489604</v>
       </c>
       <c r="M525">
         <v>2766</v>
       </c>
       <c r="N525" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.36357481381178E-2</v>
       </c>
       <c r="O525">
@@ -23727,7 +23727,7 @@
         <v>15986</v>
       </c>
     </row>
-    <row r="526" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="526" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A526">
         <v>2021</v>
       </c>
@@ -23744,7 +23744,7 @@
         <v>68</v>
       </c>
       <c r="F526" s="3">
-        <f>SUM(Q526/129293)</f>
+        <f t="shared" si="0"/>
         <v>2.5678110957283069E-2</v>
       </c>
       <c r="G526" t="s">
@@ -23760,7 +23760,7 @@
         <v>274</v>
       </c>
       <c r="K526" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.5471698113207548E-3</v>
       </c>
       <c r="L526" s="4">
@@ -23770,7 +23770,7 @@
         <v>901</v>
       </c>
       <c r="N526" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.0501015572105619E-2</v>
       </c>
       <c r="O526">
@@ -23783,7 +23783,7 @@
         <v>3320</v>
       </c>
     </row>
-    <row r="527" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="527" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A527">
         <v>2021</v>
       </c>
@@ -23800,7 +23800,7 @@
         <v>76</v>
       </c>
       <c r="F527" s="3">
-        <f>SUM(Q527/129293)</f>
+        <f t="shared" si="0"/>
         <v>1.672170960531506E-2</v>
       </c>
       <c r="G527" t="s">
@@ -23816,7 +23816,7 @@
         <v>1570</v>
       </c>
       <c r="K527" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.3244732130560529E-2</v>
       </c>
       <c r="L527" s="4">
@@ -23826,7 +23826,7 @@
         <v>0</v>
       </c>
       <c r="N527" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O527">
@@ -23839,7 +23839,7 @@
         <v>2162</v>
       </c>
     </row>
-    <row r="528" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="528" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A528">
         <v>2021</v>
       </c>
@@ -23856,7 +23856,7 @@
         <v>87</v>
       </c>
       <c r="F528" s="3">
-        <f>SUM(Q528/129293)</f>
+        <f t="shared" si="0"/>
         <v>3.3103106896738413E-2</v>
       </c>
       <c r="G528" t="s">
@@ -23872,18 +23872,18 @@
         <v>2046</v>
       </c>
       <c r="K528" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.6355873846577607E-2</v>
       </c>
       <c r="L528" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.77964467704173</v>
       </c>
       <c r="M528">
         <v>2130</v>
       </c>
       <c r="N528" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.2105619498984433E-2</v>
       </c>
       <c r="O528">
@@ -23896,7 +23896,7 @@
         <v>4280</v>
       </c>
     </row>
-    <row r="529" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A529">
         <v>2021</v>
       </c>
@@ -23913,7 +23913,7 @@
         <v>118</v>
       </c>
       <c r="F529" s="3">
-        <f>SUM(Q529/129293)</f>
+        <f t="shared" si="0"/>
         <v>2.209709729064992E-2</v>
       </c>
       <c r="G529" t="s">
@@ -23929,18 +23929,18 @@
         <v>2344</v>
       </c>
       <c r="K529" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.456410962677317E-2</v>
       </c>
       <c r="L529" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18.077950695496487</v>
       </c>
       <c r="M529">
         <v>313</v>
       </c>
       <c r="N529" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.059580230196344E-2</v>
       </c>
       <c r="O529">
@@ -23953,7 +23953,7 @@
         <v>2857</v>
       </c>
     </row>
-    <row r="530" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="530" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A530">
         <v>2021</v>
       </c>
@@ -23970,7 +23970,7 @@
         <v>128</v>
       </c>
       <c r="F530" s="3">
-        <f>SUM(Q530/129293)</f>
+        <f t="shared" si="0"/>
         <v>1.0348588090615889E-2</v>
       </c>
       <c r="G530" t="s">
@@ -23986,7 +23986,7 @@
         <v>751</v>
       </c>
       <c r="K530" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0685855942707616E-2</v>
       </c>
       <c r="L530" s="4">
@@ -23996,7 +23996,7 @@
         <v>5</v>
       </c>
       <c r="N530" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6926201760324982E-4</v>
       </c>
       <c r="O530">
@@ -24009,7 +24009,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="531" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="531" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A531">
         <v>2021</v>
       </c>
@@ -24026,7 +24026,7 @@
         <v>132</v>
       </c>
       <c r="F531" s="3">
-        <f>SUM(Q531/129293)</f>
+        <f t="shared" si="0"/>
         <v>3.2739591470535914E-2</v>
       </c>
       <c r="G531" t="s">
@@ -24042,7 +24042,7 @@
         <v>164</v>
       </c>
       <c r="K531" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.5172841206445394E-3</v>
       </c>
       <c r="L531" s="4">
@@ -24052,7 +24052,7 @@
         <v>15</v>
       </c>
       <c r="N531" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.077860528097495E-4</v>
       </c>
       <c r="O531">
@@ -24065,7 +24065,7 @@
         <v>4233</v>
       </c>
     </row>
-    <row r="532" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="532" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A532">
         <v>2021</v>
       </c>
@@ -24082,7 +24082,7 @@
         <v>149</v>
       </c>
       <c r="F532" s="3">
-        <f>SUM(Q532/129293)</f>
+        <f t="shared" si="0"/>
         <v>1.8431005545543843E-2</v>
       </c>
       <c r="G532" t="s">
@@ -24098,7 +24098,7 @@
         <v>5</v>
       </c>
       <c r="K532" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3772207684891889E-4</v>
       </c>
       <c r="L532" s="4">
@@ -24108,7 +24108,7 @@
         <v>0</v>
       </c>
       <c r="N532" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O532">
@@ -24121,7 +24121,7 @@
         <v>2383</v>
       </c>
     </row>
-    <row r="533" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A533">
         <v>2021</v>
       </c>
@@ -24138,7 +24138,7 @@
         <v>143</v>
       </c>
       <c r="F533" s="3">
-        <f>SUM(Q533/129293)</f>
+        <f t="shared" si="0"/>
         <v>5.738903111537361E-3</v>
       </c>
       <c r="G533" t="s">
@@ -24154,7 +24154,7 @@
         <v>703</v>
       </c>
       <c r="K533" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9363724004957995E-2</v>
       </c>
       <c r="L533" s="4">
@@ -24164,7 +24164,7 @@
         <v>39</v>
       </c>
       <c r="N533" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3202437373053487E-3</v>
       </c>
       <c r="O533">
@@ -24177,7 +24177,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="534" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="534" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A534">
         <v>2021</v>
       </c>
@@ -24194,7 +24194,7 @@
         <v>151</v>
       </c>
       <c r="F534" s="3">
-        <f>SUM(Q534/129293)</f>
+        <f t="shared" si="0"/>
         <v>5.0737472252944862E-3</v>
       </c>
       <c r="G534" t="s">
@@ -24210,7 +24210,7 @@
         <v>70</v>
       </c>
       <c r="K534" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9281090758848643E-3</v>
       </c>
       <c r="L534" s="4">
@@ -24220,7 +24220,7 @@
         <v>5</v>
       </c>
       <c r="N534" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6926201760324982E-4</v>
       </c>
       <c r="O534">
@@ -24233,7 +24233,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="535" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="535" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A535">
         <v>2021</v>
       </c>
@@ -24250,7 +24250,7 @@
         <v>153</v>
       </c>
       <c r="F535" s="3">
-        <f>SUM(Q535/129293)</f>
+        <f t="shared" si="0"/>
         <v>2.130819147208279E-2</v>
       </c>
       <c r="G535" t="s">
@@ -24266,7 +24266,7 @@
         <v>446</v>
       </c>
       <c r="K535" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2284809254923564E-2</v>
       </c>
       <c r="L535" s="4">
@@ -24276,7 +24276,7 @@
         <v>1524</v>
       </c>
       <c r="N535" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.1591062965470551E-2</v>
       </c>
       <c r="O535">
@@ -24289,7 +24289,7 @@
         <v>2755</v>
       </c>
     </row>
-    <row r="536" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="536" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A536">
         <v>2021</v>
       </c>
@@ -24306,7 +24306,7 @@
         <v>161</v>
       </c>
       <c r="F536" s="3">
-        <f>SUM(Q536/129293)</f>
+        <f t="shared" si="0"/>
         <v>0.10803369091907528</v>
       </c>
       <c r="G536" t="s">
@@ -24322,18 +24322,18 @@
         <v>4340</v>
       </c>
       <c r="K536" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.11954276270486158</v>
       </c>
       <c r="L536" s="4">
+        <f t="shared" si="3"/>
+        <v>33.471973557361245</v>
+      </c>
+      <c r="M536">
+        <v>0</v>
+      </c>
+      <c r="N536" s="3">
         <f t="shared" si="2"/>
-        <v>33.471973557361245</v>
-      </c>
-      <c r="M536">
-        <v>0</v>
-      </c>
-      <c r="N536" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O536">
@@ -24346,7 +24346,7 @@
         <v>13968</v>
       </c>
     </row>
-    <row r="537" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="537" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A537">
         <v>2021</v>
       </c>
@@ -24363,7 +24363,7 @@
         <v>159</v>
       </c>
       <c r="F537" s="3">
-        <f>SUM(Q537/129293)</f>
+        <f t="shared" si="0"/>
         <v>2.8887874826943456E-2</v>
       </c>
       <c r="G537" t="s">
@@ -24379,18 +24379,18 @@
         <v>3675</v>
       </c>
       <c r="K537" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.10122572648395538</v>
       </c>
       <c r="L537" s="4">
+        <f t="shared" si="3"/>
+        <v>28.343203415507507</v>
+      </c>
+      <c r="M537">
+        <v>0</v>
+      </c>
+      <c r="N537" s="3">
         <f t="shared" si="2"/>
-        <v>28.343203415507507</v>
-      </c>
-      <c r="M537">
-        <v>0</v>
-      </c>
-      <c r="N537" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O537">
@@ -24403,7 +24403,7 @@
         <v>3735</v>
       </c>
     </row>
-    <row r="538" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="538" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A538">
         <v>2021</v>
       </c>
@@ -24420,7 +24420,7 @@
         <v>61</v>
       </c>
       <c r="F538" s="3">
-        <f>SUM(Q538/129293)</f>
+        <f t="shared" si="0"/>
         <v>8.1056205672387516E-3</v>
       </c>
       <c r="G538" t="s">
@@ -24436,7 +24436,7 @@
         <v>792</v>
       </c>
       <c r="K538" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1815176972868749E-2</v>
       </c>
       <c r="L538" s="4">
@@ -24446,7 +24446,7 @@
         <v>32</v>
       </c>
       <c r="N538" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0832769126607989E-3</v>
       </c>
       <c r="O538">
@@ -24476,7 +24476,7 @@
         <v>151</v>
       </c>
       <c r="F539" s="3">
-        <f>SUM(Q539/129293)</f>
+        <f t="shared" si="0"/>
         <v>4.2539039236462921E-3</v>
       </c>
       <c r="G539" t="s">
@@ -24521,7 +24521,7 @@
         <v>57</v>
       </c>
       <c r="F540" s="3">
-        <f>SUM(Q540/129293)</f>
+        <f t="shared" si="0"/>
         <v>3.6042167789439492E-3</v>
       </c>
       <c r="G540" t="s">
@@ -24566,7 +24566,7 @@
         <v>136</v>
       </c>
       <c r="F541" s="3">
-        <f>SUM(Q541/129293)</f>
+        <f t="shared" si="0"/>
         <v>3.6042167789439492E-3</v>
       </c>
       <c r="G541" t="s">
@@ -24611,7 +24611,7 @@
         <v>43</v>
       </c>
       <c r="F542" s="3">
-        <f>SUM(Q542/129293)</f>
+        <f t="shared" si="0"/>
         <v>3.5423418127818211E-3</v>
       </c>
       <c r="G542" t="s">
@@ -24656,7 +24656,7 @@
         <v>61</v>
       </c>
       <c r="F543" s="3">
-        <f>SUM(Q543/129293)</f>
+        <f t="shared" si="0"/>
         <v>3.055076454255064E-3</v>
       </c>
       <c r="G543" t="s">
@@ -24701,7 +24701,7 @@
         <v>165</v>
       </c>
       <c r="F544" s="3">
-        <f>SUM(Q544/129293)</f>
+        <f t="shared" si="0"/>
         <v>1.9490614341070283E-3</v>
       </c>
       <c r="G544" t="s">
@@ -24746,7 +24746,7 @@
         <v>112</v>
       </c>
       <c r="F545" s="3">
-        <f>SUM(Q545/129293)</f>
+        <f t="shared" si="0"/>
         <v>1.8949208387151664E-3</v>
       </c>
       <c r="G545" t="s">
@@ -24791,7 +24791,7 @@
         <v>57</v>
       </c>
       <c r="F546" s="3">
-        <f>SUM(Q546/129293)</f>
+        <f t="shared" si="0"/>
         <v>1.8562489848638363E-3</v>
       </c>
       <c r="G546" t="s">
@@ -24836,7 +24836,7 @@
         <v>151</v>
       </c>
       <c r="F547" s="3">
-        <f>SUM(Q547/129293)</f>
+        <f t="shared" si="0"/>
         <v>1.7015615694585167E-3</v>
       </c>
       <c r="G547" t="s">
@@ -24881,7 +24881,7 @@
         <v>80</v>
       </c>
       <c r="F548" s="3">
-        <f>SUM(Q548/129293)</f>
+        <f t="shared" ref="F548:F579" si="4">SUM(Q548/129293)</f>
         <v>1.6783584571477188E-3</v>
       </c>
       <c r="G548" t="s">
@@ -24926,7 +24926,7 @@
         <v>163</v>
       </c>
       <c r="F549" s="3">
-        <f>SUM(Q549/129293)</f>
+        <f t="shared" si="4"/>
         <v>1.5314054125126651E-3</v>
       </c>
       <c r="G549" t="s">
@@ -24971,7 +24971,7 @@
         <v>24</v>
       </c>
       <c r="F550" s="3">
-        <f>SUM(Q550/129293)</f>
+        <f t="shared" si="4"/>
         <v>1.4849991878910691E-3</v>
       </c>
       <c r="G550" t="s">
@@ -25016,7 +25016,7 @@
         <v>120</v>
       </c>
       <c r="F551" s="3">
-        <f>SUM(Q551/129293)</f>
+        <f t="shared" si="4"/>
         <v>1.3689836263370793E-3</v>
       </c>
       <c r="G551" t="s">
@@ -25061,7 +25061,7 @@
         <v>78</v>
       </c>
       <c r="F552" s="3">
-        <f>SUM(Q552/129293)</f>
+        <f t="shared" si="4"/>
         <v>1.1292181324588338E-3</v>
       </c>
       <c r="G552" t="s">
@@ -25106,7 +25106,7 @@
         <v>51</v>
       </c>
       <c r="F553" s="3">
-        <f>SUM(Q553/129293)</f>
+        <f t="shared" si="4"/>
         <v>1.1214837616885678E-3</v>
       </c>
       <c r="G553" t="s">
@@ -25151,7 +25151,7 @@
         <v>104</v>
       </c>
       <c r="F554" s="3">
-        <f>SUM(Q554/129293)</f>
+        <f t="shared" si="4"/>
         <v>1.1214837616885678E-3</v>
       </c>
       <c r="G554" t="s">
@@ -25196,7 +25196,7 @@
         <v>132</v>
       </c>
       <c r="F555" s="3">
-        <f>SUM(Q555/129293)</f>
+        <f t="shared" si="4"/>
         <v>1.1214837616885678E-3</v>
       </c>
       <c r="G555" t="s">
@@ -25241,7 +25241,7 @@
         <v>30</v>
       </c>
       <c r="F556" s="3">
-        <f>SUM(Q556/129293)</f>
+        <f t="shared" si="4"/>
         <v>1.051874424756174E-3</v>
       </c>
       <c r="G556" t="s">
@@ -25286,7 +25286,7 @@
         <v>76</v>
       </c>
       <c r="F557" s="3">
-        <f>SUM(Q557/129293)</f>
+        <f t="shared" si="4"/>
         <v>1.044140053985908E-3</v>
       </c>
       <c r="G557" t="s">
@@ -25331,7 +25331,7 @@
         <v>118</v>
       </c>
       <c r="F558" s="3">
-        <f>SUM(Q558/129293)</f>
+        <f t="shared" si="4"/>
         <v>1.0209369416751099E-3</v>
       </c>
       <c r="G558" t="s">
@@ -25376,7 +25376,7 @@
         <v>89</v>
       </c>
       <c r="F559" s="3">
-        <f>SUM(Q559/129293)</f>
+        <f t="shared" si="4"/>
         <v>9.203901216616522E-4</v>
       </c>
       <c r="G559" t="s">
@@ -25421,7 +25421,7 @@
         <v>130</v>
       </c>
       <c r="F560" s="3">
-        <f>SUM(Q560/129293)</f>
+        <f t="shared" si="4"/>
         <v>7.8117144779686447E-4</v>
       </c>
       <c r="G560" t="s">
@@ -25466,7 +25466,7 @@
         <v>114</v>
       </c>
       <c r="F561" s="3">
-        <f>SUM(Q561/129293)</f>
+        <f t="shared" si="4"/>
         <v>7.5796833548606658E-4</v>
       </c>
       <c r="G561" t="s">
@@ -25511,7 +25511,7 @@
         <v>24</v>
       </c>
       <c r="F562" s="3">
-        <f>SUM(Q562/129293)</f>
+        <f t="shared" si="4"/>
         <v>6.2648403239154481E-4</v>
       </c>
       <c r="G562" t="s">
@@ -25556,7 +25556,7 @@
         <v>147</v>
       </c>
       <c r="F563" s="3">
-        <f>SUM(Q563/129293)</f>
+        <f t="shared" si="4"/>
         <v>5.7234343699968286E-4</v>
       </c>
       <c r="G563" t="s">
@@ -25601,7 +25601,7 @@
         <v>43</v>
       </c>
       <c r="F564" s="3">
-        <f>SUM(Q564/129293)</f>
+        <f t="shared" si="4"/>
         <v>5.4914032468888498E-4</v>
       </c>
       <c r="G564" t="s">
@@ -25646,7 +25646,7 @@
         <v>74</v>
       </c>
       <c r="F565" s="3">
-        <f>SUM(Q565/129293)</f>
+        <f t="shared" si="4"/>
         <v>5.4914032468888498E-4</v>
       </c>
       <c r="G565" t="s">
@@ -25691,7 +25691,7 @@
         <v>120</v>
       </c>
       <c r="F566" s="3">
-        <f>SUM(Q566/129293)</f>
+        <f t="shared" si="4"/>
         <v>5.3367158314835295E-4</v>
       </c>
       <c r="G566" t="s">
@@ -25736,7 +25736,7 @@
         <v>136</v>
       </c>
       <c r="F567" s="3">
-        <f>SUM(Q567/129293)</f>
+        <f t="shared" si="4"/>
         <v>3.557810554322353E-4</v>
       </c>
       <c r="G567" t="s">
@@ -25781,7 +25781,7 @@
         <v>145</v>
       </c>
       <c r="F568" s="3">
-        <f>SUM(Q568/129293)</f>
+        <f t="shared" si="4"/>
         <v>3.4804668466196934E-4</v>
       </c>
       <c r="G568" t="s">
@@ -25826,7 +25826,7 @@
         <v>53</v>
       </c>
       <c r="F569" s="3">
-        <f>SUM(Q569/129293)</f>
+        <f t="shared" si="4"/>
         <v>3.2484357235117135E-4</v>
       </c>
       <c r="G569" t="s">
@@ -25871,7 +25871,7 @@
         <v>94</v>
       </c>
       <c r="F570" s="3">
-        <f>SUM(Q570/129293)</f>
+        <f t="shared" si="4"/>
         <v>3.0937483081063942E-4</v>
       </c>
       <c r="G570" t="s">
@@ -25916,7 +25916,7 @@
         <v>169</v>
       </c>
       <c r="F571" s="3">
-        <f>SUM(Q571/129293)</f>
+        <f t="shared" si="4"/>
         <v>2.6296860618904349E-4</v>
       </c>
       <c r="G571" t="s">
@@ -25961,7 +25961,7 @@
         <v>53</v>
       </c>
       <c r="F572" s="3">
-        <f>SUM(Q572/129293)</f>
+        <f t="shared" si="4"/>
         <v>2.6296860618904349E-4</v>
       </c>
       <c r="G572" t="s">
@@ -26006,7 +26006,7 @@
         <v>163</v>
       </c>
       <c r="F573" s="3">
-        <f>SUM(Q573/129293)</f>
+        <f t="shared" si="4"/>
         <v>2.5523423541877748E-4</v>
       </c>
       <c r="G573" t="s">
@@ -26051,7 +26051,7 @@
         <v>112</v>
       </c>
       <c r="F574" s="3">
-        <f>SUM(Q574/129293)</f>
+        <f t="shared" si="4"/>
         <v>2.1656238156744759E-4</v>
       </c>
       <c r="G574" t="s">
@@ -26096,7 +26096,7 @@
         <v>106</v>
       </c>
       <c r="F575" s="3">
-        <f>SUM(Q575/129293)</f>
+        <f t="shared" si="4"/>
         <v>2.088280107971816E-4</v>
       </c>
       <c r="G575" t="s">
@@ -26141,7 +26141,7 @@
         <v>157</v>
       </c>
       <c r="F576" s="3">
-        <f>SUM(Q576/129293)</f>
+        <f t="shared" si="4"/>
         <v>1.7789052771611765E-4</v>
       </c>
       <c r="G576" t="s">
@@ -26186,7 +26186,7 @@
         <v>165</v>
       </c>
       <c r="F577" s="3">
-        <f>SUM(Q577/129293)</f>
+        <f t="shared" si="4"/>
         <v>1.7789052771611765E-4</v>
       </c>
       <c r="G577" t="s">
@@ -26231,7 +26231,7 @@
         <v>37</v>
       </c>
       <c r="F578" s="3">
-        <f>SUM(Q578/129293)</f>
+        <f t="shared" si="4"/>
         <v>1.7015615694585166E-4</v>
       </c>
       <c r="G578" t="s">
@@ -26276,7 +26276,7 @@
         <v>124</v>
       </c>
       <c r="F579" s="3">
-        <f>SUM(Q579/129293)</f>
+        <f t="shared" si="4"/>
         <v>1.6242178617558567E-4</v>
       </c>
       <c r="G579" t="s">
@@ -26321,7 +26321,7 @@
         <v>72</v>
       </c>
       <c r="F580" s="3">
-        <f>SUM(Q580/129293)</f>
+        <f t="shared" ref="F580:F611" si="5">SUM(Q580/129293)</f>
         <v>1.4695304463505372E-4</v>
       </c>
       <c r="G580" t="s">
@@ -26366,7 +26366,7 @@
         <v>122</v>
       </c>
       <c r="F581" s="3">
-        <f>SUM(Q581/129293)</f>
+        <f t="shared" si="5"/>
         <v>1.3921867386478774E-4</v>
       </c>
       <c r="G581" t="s">
@@ -26411,7 +26411,7 @@
         <v>55</v>
       </c>
       <c r="F582" s="3">
-        <f>SUM(Q582/129293)</f>
+        <f t="shared" si="5"/>
         <v>1.1601556155398977E-4</v>
       </c>
       <c r="G582" t="s">
@@ -26456,7 +26456,7 @@
         <v>155</v>
       </c>
       <c r="F583" s="3">
-        <f>SUM(Q583/129293)</f>
+        <f t="shared" si="5"/>
         <v>1.1601556155398977E-4</v>
       </c>
       <c r="G583" t="s">
@@ -26501,7 +26501,7 @@
         <v>171</v>
       </c>
       <c r="F584" s="3">
-        <f>SUM(Q584/129293)</f>
+        <f t="shared" si="5"/>
         <v>1.082811907837238E-4</v>
       </c>
       <c r="G584" t="s">
@@ -26546,7 +26546,7 @@
         <v>63</v>
       </c>
       <c r="F585" s="3">
-        <f>SUM(Q585/129293)</f>
+        <f t="shared" si="5"/>
         <v>1.082811907837238E-4</v>
       </c>
       <c r="G585" t="s">
@@ -26591,7 +26591,7 @@
         <v>74</v>
       </c>
       <c r="F586" s="3">
-        <f>SUM(Q586/129293)</f>
+        <f t="shared" si="5"/>
         <v>1.0054682001345781E-4</v>
       </c>
       <c r="G586" t="s">
@@ -26636,7 +26636,7 @@
         <v>185</v>
       </c>
       <c r="F587" s="3">
-        <f>SUM(Q587/129293)</f>
+        <f t="shared" si="5"/>
         <v>8.5078078472925831E-5</v>
       </c>
       <c r="G587" t="s">
@@ -26681,7 +26681,7 @@
         <v>89</v>
       </c>
       <c r="F588" s="3">
-        <f>SUM(Q588/129293)</f>
+        <f t="shared" si="5"/>
         <v>8.5078078472925831E-5</v>
       </c>
       <c r="G588" t="s">
@@ -26726,7 +26726,7 @@
         <v>30</v>
       </c>
       <c r="F589" s="3">
-        <f>SUM(Q589/129293)</f>
+        <f t="shared" si="5"/>
         <v>7.7343707702659856E-5</v>
       </c>
       <c r="G589" t="s">
@@ -26771,7 +26771,7 @@
         <v>169</v>
       </c>
       <c r="F590" s="3">
-        <f>SUM(Q590/129293)</f>
+        <f t="shared" si="5"/>
         <v>7.7343707702659856E-5</v>
       </c>
       <c r="G590" t="s">
@@ -26816,7 +26816,7 @@
         <v>39</v>
       </c>
       <c r="F591" s="3">
-        <f>SUM(Q591/129293)</f>
+        <f t="shared" si="5"/>
         <v>7.7343707702659856E-5</v>
       </c>
       <c r="G591" t="s">
@@ -26861,7 +26861,7 @@
         <v>21</v>
       </c>
       <c r="F592" s="3">
-        <f>SUM(Q592/129293)</f>
+        <f t="shared" si="5"/>
         <v>7.7343707702659856E-5</v>
       </c>
       <c r="G592" t="s">
@@ -26906,7 +26906,7 @@
         <v>104</v>
       </c>
       <c r="F593" s="3">
-        <f>SUM(Q593/129293)</f>
+        <f t="shared" si="5"/>
         <v>7.7343707702659856E-5</v>
       </c>
       <c r="G593" t="s">
@@ -26951,7 +26951,7 @@
         <v>177</v>
       </c>
       <c r="F594" s="3">
-        <f>SUM(Q594/129293)</f>
+        <f t="shared" si="5"/>
         <v>7.7343707702659856E-5</v>
       </c>
       <c r="G594" t="s">
@@ -26996,7 +26996,7 @@
         <v>108</v>
       </c>
       <c r="F595" s="3">
-        <f>SUM(Q595/129293)</f>
+        <f t="shared" si="5"/>
         <v>7.7343707702659856E-5</v>
       </c>
       <c r="G595" t="s">
@@ -27041,7 +27041,7 @@
         <v>61</v>
       </c>
       <c r="F596" s="3">
-        <f>SUM(Q596/129293)</f>
+        <f t="shared" si="5"/>
         <v>7.7343707702659856E-5</v>
       </c>
       <c r="G596" t="s">
@@ -27086,7 +27086,7 @@
         <v>165</v>
       </c>
       <c r="F597" s="3">
-        <f>SUM(Q597/129293)</f>
+        <f t="shared" si="5"/>
         <v>7.7343707702659856E-5</v>
       </c>
       <c r="G597" t="s">
@@ -27131,7 +27131,7 @@
         <v>16</v>
       </c>
       <c r="F598" s="3">
-        <f>SUM(Q598/129293)</f>
+        <f t="shared" si="5"/>
         <v>3.8671853851329928E-5</v>
       </c>
       <c r="G598" t="s">
@@ -27176,7 +27176,7 @@
         <v>183</v>
       </c>
       <c r="F599" s="3">
-        <f>SUM(Q599/129293)</f>
+        <f t="shared" si="5"/>
         <v>3.8671853851329928E-5</v>
       </c>
       <c r="G599" t="s">
@@ -27221,7 +27221,7 @@
         <v>70</v>
       </c>
       <c r="F600" s="3">
-        <f>SUM(Q600/129293)</f>
+        <f t="shared" si="5"/>
         <v>3.8671853851329928E-5</v>
       </c>
       <c r="G600" t="s">
@@ -27266,7 +27266,7 @@
         <v>49</v>
       </c>
       <c r="F601" s="3">
-        <f>SUM(Q601/129293)</f>
+        <f t="shared" si="5"/>
         <v>3.8671853851329928E-5</v>
       </c>
       <c r="G601" t="s">
@@ -27311,7 +27311,7 @@
         <v>80</v>
       </c>
       <c r="F602" s="3">
-        <f>SUM(Q602/129293)</f>
+        <f t="shared" si="5"/>
         <v>3.8671853851329928E-5</v>
       </c>
       <c r="G602" t="s">
@@ -27356,7 +27356,7 @@
         <v>91</v>
       </c>
       <c r="F603" s="3">
-        <f>SUM(Q603/129293)</f>
+        <f t="shared" si="5"/>
         <v>3.8671853851329928E-5</v>
       </c>
       <c r="G603" t="s">
@@ -27401,7 +27401,7 @@
         <v>98</v>
       </c>
       <c r="F604" s="3">
-        <f>SUM(Q604/129293)</f>
+        <f t="shared" si="5"/>
         <v>3.8671853851329928E-5</v>
       </c>
       <c r="G604" t="s">
@@ -27446,7 +27446,7 @@
         <v>102</v>
       </c>
       <c r="F605" s="3">
-        <f>SUM(Q605/129293)</f>
+        <f t="shared" si="5"/>
         <v>3.8671853851329928E-5</v>
       </c>
       <c r="G605" t="s">
@@ -27491,7 +27491,7 @@
         <v>193</v>
       </c>
       <c r="F606" s="3">
-        <f>SUM(Q606/129293)</f>
+        <f t="shared" si="5"/>
         <v>3.8671853851329928E-5</v>
       </c>
       <c r="G606" t="s">
@@ -27536,7 +27536,7 @@
         <v>120</v>
       </c>
       <c r="F607" s="3">
-        <f>SUM(Q607/129293)</f>
+        <f t="shared" si="5"/>
         <v>3.8671853851329928E-5</v>
       </c>
       <c r="G607" t="s">
@@ -27581,7 +27581,7 @@
         <v>96</v>
       </c>
       <c r="F608" s="3">
-        <f>SUM(Q608/129293)</f>
+        <f t="shared" si="5"/>
         <v>3.8671853851329928E-5</v>
       </c>
       <c r="G608" t="s">
@@ -27626,7 +27626,7 @@
         <v>100</v>
       </c>
       <c r="F609" s="3">
-        <f>SUM(Q609/129293)</f>
+        <f t="shared" si="5"/>
         <v>3.8671853851329928E-5</v>
       </c>
       <c r="G609" t="s">
@@ -27671,7 +27671,7 @@
         <v>163</v>
       </c>
       <c r="F610" s="3">
-        <f>SUM(Q610/129293)</f>
+        <f t="shared" si="5"/>
         <v>3.8671853851329928E-5</v>
       </c>
       <c r="G610" t="s">
@@ -27716,7 +27716,7 @@
         <v>203</v>
       </c>
       <c r="F611" s="3">
-        <f>SUM(Q611/129293)</f>
+        <f t="shared" si="5"/>
         <v>3.8671853851329928E-5</v>
       </c>
       <c r="G611" t="s">
@@ -27802,11 +27802,6 @@
     <filterColumn colId="0">
       <filters>
         <filter val="2021"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="0%"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A516:Q538">
@@ -27821,7 +27816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52EB603C-0968-7640-BD10-BA74139AED64}">
   <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>